<commit_message>
final submission with report
downloaded from colab
</commit_message>
<xml_diff>
--- a/Assignment-1/Report.xlsx
+++ b/Assignment-1/Report.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subangkar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subangkar\Desktop\MachineLearning\Assignment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAFC582-516E-414B-95D7-61B8F5EAA752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{F7D70112-2B26-4AEB-9B57-05A68C7F174E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Telco" sheetId="1" r:id="rId1"/>
     <sheet name="Adult" sheetId="3" r:id="rId2"/>
     <sheet name="Credit" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -171,14 +170,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C87593C-C0A3-4D38-B046-875DB0548761}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,18 +507,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="26.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -540,7 +539,7 @@
         <v>99.79</v>
       </c>
       <c r="C4" s="2">
-        <v>74.73</v>
+        <v>73.88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -551,7 +550,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="2">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -562,7 +561,7 @@
         <v>100</v>
       </c>
       <c r="C6" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -595,15 +594,15 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="26.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -617,47 +616,47 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>76.2</v>
+        <v>78.430000000000007</v>
       </c>
       <c r="C14" s="2">
-        <v>76.08</v>
+        <v>77.569999999999993</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
       <c r="B15" s="2">
-        <v>79.14</v>
+        <v>78.510000000000005</v>
       </c>
       <c r="C15" s="2">
-        <v>78.28</v>
+        <v>78.569999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>79.75</v>
+        <v>79.180000000000007</v>
       </c>
       <c r="C16" s="2">
-        <v>79.209999999999994</v>
+        <v>79.06</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>80.53</v>
+        <v>79.64</v>
       </c>
       <c r="C17" s="2">
-        <v>78.64</v>
+        <v>79.489999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CCFB2D-F6F0-4C2D-BDA3-0665AA0090E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -687,18 +686,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="26.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -778,11 +777,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="26.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -796,47 +795,47 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>83.55</v>
+        <v>84.26</v>
       </c>
       <c r="C14" s="2">
-        <v>83.76</v>
+        <v>84.55</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
       <c r="B15" s="2">
-        <v>84.09</v>
+        <v>84.67</v>
       </c>
       <c r="C15" s="2">
-        <v>84.32</v>
+        <v>84.92</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>84.2</v>
+        <v>85.2</v>
       </c>
       <c r="C16" s="2">
-        <v>84.36</v>
+        <v>85.52</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>84.55</v>
+        <v>85.31</v>
       </c>
       <c r="C17" s="2">
-        <v>84.77</v>
+        <v>85.34</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E35A04-2741-418D-AE0C-2DD26B663D67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
@@ -866,18 +865,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="26.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -898,7 +897,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="2">
-        <v>99.1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -909,7 +908,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="2">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -920,7 +919,7 @@
         <v>100</v>
       </c>
       <c r="C6" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -953,15 +952,15 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="26.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -975,47 +974,47 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>99.3</v>
+        <v>99.52</v>
       </c>
       <c r="C14" s="2">
-        <v>99.37</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
       <c r="B15" s="2">
-        <v>99.3</v>
+        <v>99.52</v>
       </c>
       <c r="C15" s="2">
-        <v>99.37</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>99.36</v>
+        <v>99.52</v>
       </c>
       <c r="C16" s="2">
-        <v>99.44</v>
+        <v>99.46</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>99.38</v>
+        <v>99.54</v>
       </c>
       <c r="C17" s="2">
-        <v>99.41</v>
+        <v>99.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>